<commit_message>
fixed and updated the format implementation in the worbyn version
</commit_message>
<xml_diff>
--- a/FORMAT_WORBYN_2.xlsx
+++ b/FORMAT_WORBYN_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shri Karthik\Desktop\DIAGRAM-MAPPER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F56DED-623F-470D-9AB9-BDBEBC58CDAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060562E8-EC6D-4B08-9B3F-15478E002A0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FAIR" sheetId="2" r:id="rId1"/>
@@ -124,7 +124,7 @@
     <definedName name="_Dist_Bin" hidden="1">#REF!</definedName>
     <definedName name="_Dist_Values" hidden="1">#REF!</definedName>
     <definedName name="_Fill" hidden="1">'[5]SAMPLE HISTOGRAM'!$P$19:$P$28</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FAIR!$A$9:$H$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FAIR!$A$9:$H$48</definedName>
     <definedName name="_FLD1">#REF!</definedName>
     <definedName name="_FLD2">#REF!</definedName>
     <definedName name="_FLD3">#REF!</definedName>
@@ -445,7 +445,7 @@
     <definedName name="Percent_R___R_2_4">NA()</definedName>
     <definedName name="Percent_R___R_2_5">NA()</definedName>
     <definedName name="pqr">OFFSET('[7]MSA (GUAGE R R)'!#REF!,0,0,COUNT(('[7]MSA (GUAGE R R)'!#REF!))+1)</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">FAIR!$A$3:$N$49</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">FAIR!$A$3:$N$48</definedName>
     <definedName name="_xlnm.Print_Area" hidden="1">'[16]Blank Form'!$B$1:$R$40</definedName>
     <definedName name="Print_Area_MI">#REF!</definedName>
     <definedName name="Print_Area_MI_1">NA()</definedName>
@@ -1255,7 +1255,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1390,50 +1390,41 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1507,59 +1498,50 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1578,6 +1560,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -7512,11 +7506,11 @@
   <sheetPr codeName="Sheet2">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Y185"/>
+  <dimension ref="A1:Y184"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showWhiteSpace="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G40" sqref="G40"/>
+      <pane ySplit="9" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B46" sqref="B46:L46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -8232,57 +8226,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="83" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="55" t="s">
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="89" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="55"/>
+      <c r="K1" s="89"/>
       <c r="L1" s="24" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="51"/>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="56" t="s">
+      <c r="A2" s="85"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="56"/>
+      <c r="K2" s="90"/>
       <c r="L2" s="23" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:25" s="4" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="53"/>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="57" t="s">
+      <c r="A3" s="87"/>
+      <c r="B3" s="88"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="91" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="57"/>
+      <c r="K3" s="91"/>
       <c r="L3" s="33">
         <v>45901</v>
       </c>
@@ -8292,19 +8286,19 @@
         <v>15</v>
       </c>
       <c r="B4" s="27"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="62"/>
+      <c r="C4" s="94"/>
+      <c r="D4" s="95"/>
+      <c r="E4" s="95"/>
+      <c r="F4" s="96"/>
       <c r="G4" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="58" t="s">
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="59"/>
+      <c r="K4" s="93"/>
       <c r="L4" s="28"/>
     </row>
     <row r="5" spans="1:25" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -8312,19 +8306,19 @@
         <v>32</v>
       </c>
       <c r="B5" s="35"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
       <c r="G5" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="66"/>
-      <c r="I5" s="66"/>
-      <c r="J5" s="83" t="s">
+      <c r="H5" s="64"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="81" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="84"/>
+      <c r="K5" s="82"/>
       <c r="L5" s="29"/>
     </row>
     <row r="6" spans="1:25" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -8332,19 +8326,19 @@
         <v>12</v>
       </c>
       <c r="B6" s="35"/>
-      <c r="C6" s="66"/>
-      <c r="D6" s="66"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="66"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
       <c r="G6" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="66"/>
-      <c r="I6" s="66"/>
-      <c r="J6" s="83" t="s">
+      <c r="H6" s="64"/>
+      <c r="I6" s="64"/>
+      <c r="J6" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="K6" s="84"/>
+      <c r="K6" s="82"/>
       <c r="L6" s="29"/>
     </row>
     <row r="7" spans="1:25" s="4" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8352,19 +8346,19 @@
         <v>11</v>
       </c>
       <c r="B7" s="31"/>
-      <c r="C7" s="80"/>
-      <c r="D7" s="81"/>
-      <c r="E7" s="81"/>
-      <c r="F7" s="82"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="79"/>
+      <c r="E7" s="79"/>
+      <c r="F7" s="80"/>
       <c r="G7" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="67"/>
-      <c r="I7" s="67"/>
-      <c r="J7" s="76" t="s">
+      <c r="H7" s="65"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="77"/>
+      <c r="K7" s="75"/>
       <c r="L7" s="32"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
@@ -8380,32 +8374,32 @@
       <c r="Y7" s="17"/>
     </row>
     <row r="8" spans="1:25" s="4" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="69"/>
-      <c r="C8" s="69"/>
-      <c r="D8" s="69"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="69"/>
-      <c r="G8" s="69"/>
-      <c r="H8" s="69"/>
-      <c r="I8" s="70" t="s">
+      <c r="B8" s="67"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="67"/>
+      <c r="I8" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="78" t="s">
+      <c r="J8" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="K8" s="74" t="s">
+      <c r="K8" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="L8" s="72" t="s">
+      <c r="L8" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="M8" s="63" t="s">
+      <c r="M8" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="N8" s="64"/>
+      <c r="N8" s="62"/>
       <c r="P8" s="17"/>
       <c r="Q8" s="17"/>
       <c r="R8" s="17"/>
@@ -8442,10 +8436,10 @@
       <c r="H9" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="I9" s="71"/>
-      <c r="J9" s="79"/>
-      <c r="K9" s="75"/>
-      <c r="L9" s="73"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="77"/>
+      <c r="K9" s="73"/>
+      <c r="L9" s="71"/>
       <c r="M9" s="18" t="s">
         <v>6</v>
       </c>
@@ -9075,149 +9069,143 @@
       <c r="N45" s="10"/>
       <c r="O45" s="8"/>
     </row>
-    <row r="46" spans="1:15" s="4" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="85" t="s">
+    <row r="46" spans="1:15" s="4" customFormat="1" ht="74.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="B46" s="87" t="s">
+      <c r="B46" s="105" t="s">
         <v>9</v>
       </c>
-      <c r="C46" s="87"/>
-      <c r="D46" s="87"/>
-      <c r="E46" s="87"/>
-      <c r="F46" s="87"/>
-      <c r="G46" s="87"/>
-      <c r="H46" s="87"/>
-      <c r="I46" s="87"/>
-      <c r="J46" s="87"/>
-      <c r="K46" s="87"/>
-      <c r="L46" s="87"/>
-    </row>
-    <row r="47" spans="1:15" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="86"/>
-      <c r="B47" s="88"/>
-      <c r="C47" s="89"/>
-      <c r="D47" s="89"/>
-      <c r="E47" s="89"/>
-      <c r="F47" s="89"/>
-      <c r="G47" s="89"/>
-      <c r="H47" s="89"/>
-      <c r="I47" s="89"/>
-      <c r="J47" s="89"/>
-      <c r="K47" s="89"/>
-      <c r="L47" s="90"/>
-    </row>
-    <row r="48" spans="1:15" s="4" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="94" t="s">
+      <c r="C46" s="103"/>
+      <c r="D46" s="103"/>
+      <c r="E46" s="103"/>
+      <c r="F46" s="103"/>
+      <c r="G46" s="103"/>
+      <c r="H46" s="103"/>
+      <c r="I46" s="103"/>
+      <c r="J46" s="103"/>
+      <c r="K46" s="103"/>
+      <c r="L46" s="104"/>
+      <c r="M46" s="7"/>
+      <c r="N46" s="10"/>
+      <c r="O46" s="8"/>
+    </row>
+    <row r="47" spans="1:15" s="4" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="B48" s="95"/>
-      <c r="C48" s="96"/>
-      <c r="D48" s="91" t="s">
+      <c r="B47" s="53"/>
+      <c r="C47" s="54"/>
+      <c r="D47" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="E48" s="92"/>
-      <c r="F48" s="92"/>
-      <c r="G48" s="93"/>
-      <c r="H48" s="101" t="s">
+      <c r="E47" s="50"/>
+      <c r="F47" s="50"/>
+      <c r="G47" s="51"/>
+      <c r="H47" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="I48" s="96"/>
-      <c r="J48" s="91"/>
-      <c r="K48" s="92"/>
-      <c r="L48" s="93"/>
-    </row>
-    <row r="49" spans="1:12" s="4" customFormat="1" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="97" t="s">
+      <c r="I47" s="54"/>
+      <c r="J47" s="49"/>
+      <c r="K47" s="50"/>
+      <c r="L47" s="51"/>
+    </row>
+    <row r="48" spans="1:15" s="4" customFormat="1" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="B49" s="98"/>
-      <c r="C49" s="98"/>
-      <c r="D49" s="99">
+      <c r="B48" s="56"/>
+      <c r="C48" s="56"/>
+      <c r="D48" s="57">
         <v>46042</v>
       </c>
-      <c r="E49" s="99"/>
-      <c r="F49" s="100"/>
-      <c r="G49" s="100"/>
-      <c r="H49" s="102" t="s">
+      <c r="E48" s="57"/>
+      <c r="F48" s="58"/>
+      <c r="G48" s="58"/>
+      <c r="H48" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="I49" s="102"/>
-      <c r="J49" s="99"/>
-      <c r="K49" s="100"/>
-      <c r="L49" s="100"/>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I48" s="60"/>
+      <c r="J48" s="57"/>
+      <c r="K48" s="58"/>
+      <c r="L48" s="58"/>
+    </row>
+    <row r="49" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="2"/>
+    </row>
+    <row r="50" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
       <c r="K50" s="2"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
       <c r="K51" s="2"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
       <c r="K52" s="2"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
       <c r="K53" s="2"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
       <c r="K54" s="2"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
       <c r="K55" s="2"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
       <c r="K56" s="2"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
       <c r="K57" s="2"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
       <c r="K58" s="2"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I59" s="1"/>
       <c r="J59" s="1"/>
       <c r="K59" s="2"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I60" s="1"/>
       <c r="J60" s="1"/>
       <c r="K60" s="2"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I61" s="1"/>
       <c r="J61" s="1"/>
       <c r="K61" s="2"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
       <c r="K62" s="2"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I63" s="1"/>
       <c r="J63" s="1"/>
       <c r="K63" s="2"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I64" s="1"/>
       <c r="J64" s="1"/>
       <c r="K64" s="2"/>
@@ -9760,7 +9748,7 @@
     <row r="172" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I172" s="1"/>
       <c r="J172" s="1"/>
-      <c r="K172" s="2"/>
+      <c r="K172" s="1"/>
     </row>
     <row r="173" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I173" s="1"/>
@@ -9822,23 +9810,15 @@
       <c r="J184" s="1"/>
       <c r="K184" s="1"/>
     </row>
-    <row r="185" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I185" s="1"/>
-      <c r="J185" s="1"/>
-      <c r="K185" s="1"/>
-    </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="B46:L47"/>
-    <mergeCell ref="D48:G48"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="D49:G49"/>
-    <mergeCell ref="J48:L48"/>
-    <mergeCell ref="J49:L49"/>
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="H49:I49"/>
+  <mergeCells count="31">
+    <mergeCell ref="B46:L46"/>
+    <mergeCell ref="A1:I3"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C4:F4"/>
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H5:I5"/>
@@ -9855,15 +9835,17 @@
     <mergeCell ref="C7:F7"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:I3"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="D47:G47"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="D48:G48"/>
+    <mergeCell ref="J47:L47"/>
+    <mergeCell ref="J48:L48"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="H48:I48"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
-  <conditionalFormatting sqref="L10:L45 L50:L120">
+  <conditionalFormatting sqref="L49:L119 L10:L45">
     <cfRule type="cellIs" dxfId="5" priority="427" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
@@ -9876,7 +9858,7 @@
       <formula>NOT(ISERROR(SEARCH("pass",L10)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L121:L123">
+  <conditionalFormatting sqref="L120:L122">
     <cfRule type="cellIs" dxfId="2" priority="429" stopIfTrue="1" operator="equal">
       <formula>"""Fail"""</formula>
     </cfRule>
@@ -9884,7 +9866,7 @@
       <formula>"""Pass"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N10:N45">
+  <conditionalFormatting sqref="N10:N46">
     <cfRule type="expression" dxfId="0" priority="338">
       <formula>$N10="FAIL"</formula>
     </cfRule>
@@ -9946,29 +9928,29 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="15"/>
-      <c r="B2" s="103"/>
-      <c r="C2" s="104"/>
-      <c r="D2" s="104"/>
-      <c r="E2" s="104"/>
-      <c r="F2" s="104"/>
-      <c r="G2" s="104"/>
-      <c r="H2" s="104"/>
-      <c r="I2" s="104"/>
-      <c r="J2" s="104"/>
-      <c r="K2" s="105"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="99"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
-      <c r="B3" s="106"/>
-      <c r="C3" s="107"/>
-      <c r="D3" s="107"/>
-      <c r="E3" s="107"/>
-      <c r="F3" s="107"/>
-      <c r="G3" s="107"/>
-      <c r="H3" s="107"/>
-      <c r="I3" s="107"/>
-      <c r="J3" s="107"/>
-      <c r="K3" s="108"/>
+      <c r="B3" s="100"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="101"/>
+      <c r="K3" s="102"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>

</xml_diff>